<commit_message>
Updated Visits Report TC/page
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/VisitsReportData.xlsx
+++ b/src/main/resources/testdata/VisitsReportData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oabdelhady\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\momra-e2e-tests\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8966CCC-C35F-4F01-9996-C98D00B69C1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A1F471-0063-4674-AE9F-B2E0670730E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{016F1901-991C-4FFE-80FC-606DB3BD6F14}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>TestMethodName</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>TestCaseName</t>
   </si>
 </sst>
 </file>
@@ -428,75 +431,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC479AA-86D1-40B8-BB35-6A30FD3D46AF}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
-    <col min="9" max="9" width="33" customWidth="1"/>
-    <col min="10" max="10" width="41" customWidth="1"/>
-    <col min="11" max="11" width="41.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="33" customWidth="1"/>
+    <col min="11" max="11" width="41" customWidth="1"/>
+    <col min="12" max="12" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="B1" t="s">
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
       <c r="E2">
         <v>1</v>
       </c>
@@ -516,10 +520,14 @@
         <v>1</v>
       </c>
       <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Reports TC - Test Data
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/VisitsReportData.xlsx
+++ b/src/main/resources/testdata/VisitsReportData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\momra-e2e-tests\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117340C2-53EB-404B-AAAE-7DC5CAE975F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CD91D2-9048-49E7-8A6C-7834EA851DE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{016F1901-991C-4FFE-80FC-606DB3BD6F14}"/>
+    <workbookView xWindow="7035" yWindow="3390" windowWidth="13455" windowHeight="7530" xr2:uid="{016F1901-991C-4FFE-80FC-606DB3BD6F14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>TestCaseName</t>
   </si>
   <si>
-    <t>NEW</t>
-  </si>
-  <si>
     <t>602ad14290919651d8c999e0</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>01/06/2021</t>
+  </si>
+  <si>
+    <t>جديدة</t>
   </si>
 </sst>
 </file>
@@ -460,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC479AA-86D1-40B8-BB35-6A30FD3D46AF}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,34 +523,34 @@
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E2">
         <v>920022234</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2">
         <v>920022222</v>
       </c>
       <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" t="s">
         <v>20</v>
-      </c>
-      <c r="L2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Visits Test data sheet with test method name
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/VisitsReportData.xlsx
+++ b/src/main/resources/testdata/VisitsReportData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\momra-e2e-tests\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CD91D2-9048-49E7-8A6C-7834EA851DE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF77591-B70C-42EE-AD7F-14B34B4A9468}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7035" yWindow="3390" windowWidth="13455" windowHeight="7530" xr2:uid="{016F1901-991C-4FFE-80FC-606DB3BD6F14}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{016F1901-991C-4FFE-80FC-606DB3BD6F14}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>VisitStatus</t>
   </si>
   <si>
-    <t>ValidateOnDisplayBtnFunctionality</t>
-  </si>
-  <si>
     <t>TestCaseName</t>
   </si>
   <si>
@@ -97,6 +94,10 @@
   </si>
   <si>
     <t>جديدة</t>
+  </si>
+  <si>
+    <t>ValidateOnVisitsDisplayBtnFunctionality,
+ValidateOnOfficesVisitsDisplayBtnFunctionality</t>
   </si>
 </sst>
 </file>
@@ -460,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC479AA-86D1-40B8-BB35-6A30FD3D46AF}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B4:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +486,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -518,39 +519,39 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="E2">
         <v>920022234</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>920022222</v>
       </c>
       <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" t="s">
         <v>19</v>
-      </c>
-      <c r="L2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>